<commit_message>
doc: Update model results
</commit_message>
<xml_diff>
--- a/df_describe.xlsx
+++ b/df_describe.xlsx
@@ -1,181 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="53">
-  <si>
-    <t>count</t>
-  </si>
-  <si>
-    <t>unique</t>
-  </si>
-  <si>
-    <t>top</t>
-  </si>
-  <si>
-    <t>freq</t>
-  </si>
-  <si>
-    <t>mean</t>
-  </si>
-  <si>
-    <t>std</t>
-  </si>
-  <si>
-    <t>min</t>
-  </si>
-  <si>
-    <t>25%</t>
-  </si>
-  <si>
-    <t>50%</t>
-  </si>
-  <si>
-    <t>75%</t>
-  </si>
-  <si>
-    <t>max</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>message</t>
-  </si>
-  <si>
-    <t>original</t>
-  </si>
-  <si>
-    <t>Nap fe ou konnen ke apati de jodi a sevis SMS 4636 pou enfomasyon ijan</t>
-  </si>
-  <si>
-    <t>genre</t>
-  </si>
-  <si>
-    <t>news</t>
-  </si>
-  <si>
-    <t>related</t>
-  </si>
-  <si>
-    <t>request</t>
-  </si>
-  <si>
-    <t>offer</t>
-  </si>
-  <si>
-    <t>aid_related</t>
-  </si>
-  <si>
-    <t>medical_help</t>
-  </si>
-  <si>
-    <t>medical_products</t>
-  </si>
-  <si>
-    <t>search_and_rescue</t>
-  </si>
-  <si>
-    <t>security</t>
-  </si>
-  <si>
-    <t>military</t>
-  </si>
-  <si>
-    <t>child_alone</t>
-  </si>
-  <si>
-    <t>water</t>
-  </si>
-  <si>
-    <t>food</t>
-  </si>
-  <si>
-    <t>shelter</t>
-  </si>
-  <si>
-    <t>clothing</t>
-  </si>
-  <si>
-    <t>money</t>
-  </si>
-  <si>
-    <t>missing_people</t>
-  </si>
-  <si>
-    <t>refugees</t>
-  </si>
-  <si>
-    <t>death</t>
-  </si>
-  <si>
-    <t>other_aid</t>
-  </si>
-  <si>
-    <t>infrastructure_related</t>
-  </si>
-  <si>
-    <t>transport</t>
-  </si>
-  <si>
-    <t>buildings</t>
-  </si>
-  <si>
-    <t>electricity</t>
-  </si>
-  <si>
-    <t>tools</t>
-  </si>
-  <si>
-    <t>hospitals</t>
-  </si>
-  <si>
-    <t>shops</t>
-  </si>
-  <si>
-    <t>aid_centers</t>
-  </si>
-  <si>
-    <t>other_infrastructure</t>
-  </si>
-  <si>
-    <t>weather_related</t>
-  </si>
-  <si>
-    <t>floods</t>
-  </si>
-  <si>
-    <t>storm</t>
-  </si>
-  <si>
-    <t>fire</t>
-  </si>
-  <si>
-    <t>earthquake</t>
-  </si>
-  <si>
-    <t>cold</t>
-  </si>
-  <si>
-    <t>other_weather</t>
-  </si>
-  <si>
-    <t>direct_report</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -214,7 +50,6 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -230,6 +65,74 @@
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -530,51 +433,75 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:12">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12">
-      <c r="A2" s="1" t="s">
-        <v>11</v>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>count</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>unique</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>top</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>freq</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>mean</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>std</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>min</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>25%</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>50%</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>75%</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>max</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
       </c>
       <c r="B2" t="n">
         <v>26028</v>
       </c>
-      <c r="C2" t="s"/>
-      <c r="D2" t="s"/>
-      <c r="E2" t="s"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
       <c r="F2" t="n">
         <v>15250.25695404949</v>
       </c>
@@ -597,9 +524,11 @@
         <v>30265</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
-      <c r="A3" s="1" t="s">
-        <v>12</v>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>message</t>
+        </is>
       </c>
       <c r="B3" t="n">
         <v>26028</v>
@@ -613,17 +542,19 @@
       <c r="E3" t="n">
         <v>4</v>
       </c>
-      <c r="F3" t="s"/>
-      <c r="G3" t="s"/>
-      <c r="H3" t="s"/>
-      <c r="I3" t="s"/>
-      <c r="J3" t="s"/>
-      <c r="K3" t="s"/>
-      <c r="L3" t="s"/>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="A4" s="1" t="s">
-        <v>13</v>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>original</t>
+        </is>
       </c>
       <c r="B4" t="n">
         <v>10038</v>
@@ -631,23 +562,27 @@
       <c r="C4" t="n">
         <v>9507</v>
       </c>
-      <c r="D4" t="s">
-        <v>14</v>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Nap fe ou konnen ke apati de jodi a sevis SMS 4636 pou enfomasyon ijan</t>
+        </is>
       </c>
       <c r="E4" t="n">
         <v>20</v>
       </c>
-      <c r="F4" t="s"/>
-      <c r="G4" t="s"/>
-      <c r="H4" t="s"/>
-      <c r="I4" t="s"/>
-      <c r="J4" t="s"/>
-      <c r="K4" t="s"/>
-      <c r="L4" t="s"/>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="A5" s="1" t="s">
-        <v>15</v>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>genre</t>
+        </is>
       </c>
       <c r="B5" t="n">
         <v>26028</v>
@@ -655,30 +590,34 @@
       <c r="C5" t="n">
         <v>3</v>
       </c>
-      <c r="D5" t="s">
-        <v>16</v>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>news</t>
+        </is>
       </c>
       <c r="E5" t="n">
         <v>13036</v>
       </c>
-      <c r="F5" t="s"/>
-      <c r="G5" t="s"/>
-      <c r="H5" t="s"/>
-      <c r="I5" t="s"/>
-      <c r="J5" t="s"/>
-      <c r="K5" t="s"/>
-      <c r="L5" t="s"/>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6" s="1" t="s">
-        <v>17</v>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>related</t>
+        </is>
       </c>
       <c r="B6" t="n">
         <v>26028</v>
       </c>
-      <c r="C6" t="s"/>
-      <c r="D6" t="s"/>
-      <c r="E6" t="s"/>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
       <c r="F6" t="n">
         <v>0.7647917627170739</v>
       </c>
@@ -701,16 +640,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
-      <c r="A7" s="1" t="s">
-        <v>18</v>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>request</t>
+        </is>
       </c>
       <c r="B7" t="n">
         <v>26028</v>
       </c>
-      <c r="C7" t="s"/>
-      <c r="D7" t="s"/>
-      <c r="E7" t="s"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
       <c r="F7" t="n">
         <v>0.1718918088212694</v>
       </c>
@@ -733,16 +674,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
-      <c r="A8" s="1" t="s">
-        <v>19</v>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>offer</t>
+        </is>
       </c>
       <c r="B8" t="n">
         <v>26028</v>
       </c>
-      <c r="C8" t="s"/>
-      <c r="D8" t="s"/>
-      <c r="E8" t="s"/>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
       <c r="F8" t="n">
         <v>0.004533579222375903</v>
       </c>
@@ -765,16 +708,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
-      <c r="A9" s="1" t="s">
-        <v>20</v>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>aid_related</t>
+        </is>
       </c>
       <c r="B9" t="n">
         <v>26028</v>
       </c>
-      <c r="C9" t="s"/>
-      <c r="D9" t="s"/>
-      <c r="E9" t="s"/>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
       <c r="F9" t="n">
         <v>0.417242969110189</v>
       </c>
@@ -797,16 +742,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
-      <c r="A10" s="1" t="s">
-        <v>21</v>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>medical_help</t>
+        </is>
       </c>
       <c r="B10" t="n">
         <v>26028</v>
       </c>
-      <c r="C10" t="s"/>
-      <c r="D10" t="s"/>
-      <c r="E10" t="s"/>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
       <c r="F10" t="n">
         <v>0.08006761948670663</v>
       </c>
@@ -829,16 +776,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
-      <c r="A11" s="1" t="s">
-        <v>22</v>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>medical_products</t>
+        </is>
       </c>
       <c r="B11" t="n">
         <v>26028</v>
       </c>
-      <c r="C11" t="s"/>
-      <c r="D11" t="s"/>
-      <c r="E11" t="s"/>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
       <c r="F11" t="n">
         <v>0.05044567388965729</v>
       </c>
@@ -861,16 +810,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
-      <c r="A12" s="1" t="s">
-        <v>23</v>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>search_and_rescue</t>
+        </is>
       </c>
       <c r="B12" t="n">
         <v>26028</v>
       </c>
-      <c r="C12" t="s"/>
-      <c r="D12" t="s"/>
-      <c r="E12" t="s"/>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
       <c r="F12" t="n">
         <v>0.02781619794067927</v>
       </c>
@@ -893,16 +844,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
-      <c r="A13" s="1" t="s">
-        <v>24</v>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>security</t>
+        </is>
       </c>
       <c r="B13" t="n">
         <v>26028</v>
       </c>
-      <c r="C13" t="s"/>
-      <c r="D13" t="s"/>
-      <c r="E13" t="s"/>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
       <c r="F13" t="n">
         <v>0.01809589672660212</v>
       </c>
@@ -925,16 +878,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
-      <c r="A14" s="1" t="s">
-        <v>25</v>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>military</t>
+        </is>
       </c>
       <c r="B14" t="n">
         <v>26028</v>
       </c>
-      <c r="C14" t="s"/>
-      <c r="D14" t="s"/>
-      <c r="E14" t="s"/>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
       <c r="F14" t="n">
         <v>0.03304134009528201</v>
       </c>
@@ -957,16 +912,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
-      <c r="A15" s="1" t="s">
-        <v>26</v>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>child_alone</t>
+        </is>
       </c>
       <c r="B15" t="n">
         <v>26028</v>
       </c>
-      <c r="C15" t="s"/>
-      <c r="D15" t="s"/>
-      <c r="E15" t="s"/>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
       <c r="F15" t="n">
         <v>0</v>
       </c>
@@ -989,16 +946,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
-      <c r="A16" s="1" t="s">
-        <v>27</v>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>water</t>
+        </is>
       </c>
       <c r="B16" t="n">
         <v>26028</v>
       </c>
-      <c r="C16" t="s"/>
-      <c r="D16" t="s"/>
-      <c r="E16" t="s"/>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr"/>
       <c r="F16" t="n">
         <v>0.06423851237129245</v>
       </c>
@@ -1021,16 +980,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
-      <c r="A17" s="1" t="s">
-        <v>28</v>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>food</t>
+        </is>
       </c>
       <c r="B17" t="n">
         <v>26028</v>
       </c>
-      <c r="C17" t="s"/>
-      <c r="D17" t="s"/>
-      <c r="E17" t="s"/>
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr"/>
       <c r="F17" t="n">
         <v>0.1123021361610573</v>
       </c>
@@ -1053,16 +1014,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
-      <c r="A18" s="1" t="s">
-        <v>29</v>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>shelter</t>
+        </is>
       </c>
       <c r="B18" t="n">
         <v>26028</v>
       </c>
-      <c r="C18" t="s"/>
-      <c r="D18" t="s"/>
-      <c r="E18" t="s"/>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr"/>
       <c r="F18" t="n">
         <v>0.08890425695404948</v>
       </c>
@@ -1085,16 +1048,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
-      <c r="A19" s="1" t="s">
-        <v>30</v>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>clothing</t>
+        </is>
       </c>
       <c r="B19" t="n">
         <v>26028</v>
       </c>
-      <c r="C19" t="s"/>
-      <c r="D19" t="s"/>
-      <c r="E19" t="s"/>
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="inlineStr"/>
       <c r="F19" t="n">
         <v>0.01556016597510373</v>
       </c>
@@ -1117,16 +1082,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
-      <c r="A20" s="1" t="s">
-        <v>31</v>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>money</t>
+        </is>
       </c>
       <c r="B20" t="n">
         <v>26028</v>
       </c>
-      <c r="C20" t="s"/>
-      <c r="D20" t="s"/>
-      <c r="E20" t="s"/>
+      <c r="C20" t="inlineStr"/>
+      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr"/>
       <c r="F20" t="n">
         <v>0.02320577839250038</v>
       </c>
@@ -1149,16 +1116,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
-      <c r="A21" s="1" t="s">
-        <v>32</v>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>missing_people</t>
+        </is>
       </c>
       <c r="B21" t="n">
         <v>26028</v>
       </c>
-      <c r="C21" t="s"/>
-      <c r="D21" t="s"/>
-      <c r="E21" t="s"/>
+      <c r="C21" t="inlineStr"/>
+      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr"/>
       <c r="F21" t="n">
         <v>0.01144920854464423</v>
       </c>
@@ -1181,16 +1150,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
-      <c r="A22" s="1" t="s">
-        <v>33</v>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>refugees</t>
+        </is>
       </c>
       <c r="B22" t="n">
         <v>26028</v>
       </c>
-      <c r="C22" t="s"/>
-      <c r="D22" t="s"/>
-      <c r="E22" t="s"/>
+      <c r="C22" t="inlineStr"/>
+      <c r="D22" t="inlineStr"/>
+      <c r="E22" t="inlineStr"/>
       <c r="F22" t="n">
         <v>0.03361764253880437</v>
       </c>
@@ -1213,16 +1184,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
-      <c r="A23" s="1" t="s">
-        <v>34</v>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>death</t>
+        </is>
       </c>
       <c r="B23" t="n">
         <v>26028</v>
       </c>
-      <c r="C23" t="s"/>
-      <c r="D23" t="s"/>
-      <c r="E23" t="s"/>
+      <c r="C23" t="inlineStr"/>
+      <c r="D23" t="inlineStr"/>
+      <c r="E23" t="inlineStr"/>
       <c r="F23" t="n">
         <v>0.0458736745043799</v>
       </c>
@@ -1245,16 +1218,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
-      <c r="A24" s="1" t="s">
-        <v>35</v>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>other_aid</t>
+        </is>
       </c>
       <c r="B24" t="n">
         <v>26028</v>
       </c>
-      <c r="C24" t="s"/>
-      <c r="D24" t="s"/>
-      <c r="E24" t="s"/>
+      <c r="C24" t="inlineStr"/>
+      <c r="D24" t="inlineStr"/>
+      <c r="E24" t="inlineStr"/>
       <c r="F24" t="n">
         <v>0.132395881358537</v>
       </c>
@@ -1277,16 +1252,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
-      <c r="A25" s="1" t="s">
-        <v>36</v>
+    <row r="25">
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>infrastructure_related</t>
+        </is>
       </c>
       <c r="B25" t="n">
         <v>26028</v>
       </c>
-      <c r="C25" t="s"/>
-      <c r="D25" t="s"/>
-      <c r="E25" t="s"/>
+      <c r="C25" t="inlineStr"/>
+      <c r="D25" t="inlineStr"/>
+      <c r="E25" t="inlineStr"/>
       <c r="F25" t="n">
         <v>0.06550637774704164</v>
       </c>
@@ -1309,16 +1286,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
-      <c r="A26" s="1" t="s">
-        <v>37</v>
+    <row r="26">
+      <c r="A26" s="1" t="inlineStr">
+        <is>
+          <t>transport</t>
+        </is>
       </c>
       <c r="B26" t="n">
         <v>26028</v>
       </c>
-      <c r="C26" t="s"/>
-      <c r="D26" t="s"/>
-      <c r="E26" t="s"/>
+      <c r="C26" t="inlineStr"/>
+      <c r="D26" t="inlineStr"/>
+      <c r="E26" t="inlineStr"/>
       <c r="F26" t="n">
         <v>0.04614261564469033</v>
       </c>
@@ -1341,16 +1320,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
-      <c r="A27" s="1" t="s">
-        <v>38</v>
+    <row r="27">
+      <c r="A27" s="1" t="inlineStr">
+        <is>
+          <t>buildings</t>
+        </is>
       </c>
       <c r="B27" t="n">
         <v>26028</v>
       </c>
-      <c r="C27" t="s"/>
-      <c r="D27" t="s"/>
-      <c r="E27" t="s"/>
+      <c r="C27" t="inlineStr"/>
+      <c r="D27" t="inlineStr"/>
+      <c r="E27" t="inlineStr"/>
       <c r="F27" t="n">
         <v>0.05121407714768711</v>
       </c>
@@ -1373,16 +1354,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
-      <c r="A28" s="1" t="s">
-        <v>39</v>
+    <row r="28">
+      <c r="A28" s="1" t="inlineStr">
+        <is>
+          <t>electricity</t>
+        </is>
       </c>
       <c r="B28" t="n">
         <v>26028</v>
       </c>
-      <c r="C28" t="s"/>
-      <c r="D28" t="s"/>
-      <c r="E28" t="s"/>
+      <c r="C28" t="inlineStr"/>
+      <c r="D28" t="inlineStr"/>
+      <c r="E28" t="inlineStr"/>
       <c r="F28" t="n">
         <v>0.02043952666359306</v>
       </c>
@@ -1405,16 +1388,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
-      <c r="A29" s="1" t="s">
-        <v>40</v>
+    <row r="29">
+      <c r="A29" s="1" t="inlineStr">
+        <is>
+          <t>tools</t>
+        </is>
       </c>
       <c r="B29" t="n">
         <v>26028</v>
       </c>
-      <c r="C29" t="s"/>
-      <c r="D29" t="s"/>
-      <c r="E29" t="s"/>
+      <c r="C29" t="inlineStr"/>
+      <c r="D29" t="inlineStr"/>
+      <c r="E29" t="inlineStr"/>
       <c r="F29" t="n">
         <v>0.006108805901337022</v>
       </c>
@@ -1437,16 +1422,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
-      <c r="A30" s="1" t="s">
-        <v>41</v>
+    <row r="30">
+      <c r="A30" s="1" t="inlineStr">
+        <is>
+          <t>hospitals</t>
+        </is>
       </c>
       <c r="B30" t="n">
         <v>26028</v>
       </c>
-      <c r="C30" t="s"/>
-      <c r="D30" t="s"/>
-      <c r="E30" t="s"/>
+      <c r="C30" t="inlineStr"/>
+      <c r="D30" t="inlineStr"/>
+      <c r="E30" t="inlineStr"/>
       <c r="F30" t="n">
         <v>0.01087290610112187</v>
       </c>
@@ -1469,16 +1456,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:12">
-      <c r="A31" s="1" t="s">
-        <v>42</v>
+    <row r="31">
+      <c r="A31" s="1" t="inlineStr">
+        <is>
+          <t>shops</t>
+        </is>
       </c>
       <c r="B31" t="n">
         <v>26028</v>
       </c>
-      <c r="C31" t="s"/>
-      <c r="D31" t="s"/>
-      <c r="E31" t="s"/>
+      <c r="C31" t="inlineStr"/>
+      <c r="D31" t="inlineStr"/>
+      <c r="E31" t="inlineStr"/>
       <c r="F31" t="n">
         <v>0.004610419548178884</v>
       </c>
@@ -1501,16 +1490,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:12">
-      <c r="A32" s="1" t="s">
-        <v>43</v>
+    <row r="32">
+      <c r="A32" s="1" t="inlineStr">
+        <is>
+          <t>aid_centers</t>
+        </is>
       </c>
       <c r="B32" t="n">
         <v>26028</v>
       </c>
-      <c r="C32" t="s"/>
-      <c r="D32" t="s"/>
-      <c r="E32" t="s"/>
+      <c r="C32" t="inlineStr"/>
+      <c r="D32" t="inlineStr"/>
+      <c r="E32" t="inlineStr"/>
       <c r="F32" t="n">
         <v>0.01187183033656063</v>
       </c>
@@ -1533,16 +1524,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:12">
-      <c r="A33" s="1" t="s">
-        <v>44</v>
+    <row r="33">
+      <c r="A33" s="1" t="inlineStr">
+        <is>
+          <t>other_infrastructure</t>
+        </is>
       </c>
       <c r="B33" t="n">
         <v>26028</v>
       </c>
-      <c r="C33" t="s"/>
-      <c r="D33" t="s"/>
-      <c r="E33" t="s"/>
+      <c r="C33" t="inlineStr"/>
+      <c r="D33" t="inlineStr"/>
+      <c r="E33" t="inlineStr"/>
       <c r="F33" t="n">
         <v>0.0442216074996158</v>
       </c>
@@ -1565,16 +1558,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:12">
-      <c r="A34" s="1" t="s">
-        <v>45</v>
+    <row r="34">
+      <c r="A34" s="1" t="inlineStr">
+        <is>
+          <t>weather_related</t>
+        </is>
       </c>
       <c r="B34" t="n">
         <v>26028</v>
       </c>
-      <c r="C34" t="s"/>
-      <c r="D34" t="s"/>
-      <c r="E34" t="s"/>
+      <c r="C34" t="inlineStr"/>
+      <c r="D34" t="inlineStr"/>
+      <c r="E34" t="inlineStr"/>
       <c r="F34" t="n">
         <v>0.2803519286921777</v>
       </c>
@@ -1597,16 +1592,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:12">
-      <c r="A35" s="1" t="s">
-        <v>46</v>
+    <row r="35">
+      <c r="A35" s="1" t="inlineStr">
+        <is>
+          <t>floods</t>
+        </is>
       </c>
       <c r="B35" t="n">
         <v>26028</v>
       </c>
-      <c r="C35" t="s"/>
-      <c r="D35" t="s"/>
-      <c r="E35" t="s"/>
+      <c r="C35" t="inlineStr"/>
+      <c r="D35" t="inlineStr"/>
+      <c r="E35" t="inlineStr"/>
       <c r="F35" t="n">
         <v>0.08279545105271247</v>
       </c>
@@ -1629,16 +1626,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:12">
-      <c r="A36" s="1" t="s">
-        <v>47</v>
+    <row r="36">
+      <c r="A36" s="1" t="inlineStr">
+        <is>
+          <t>storm</t>
+        </is>
       </c>
       <c r="B36" t="n">
         <v>26028</v>
       </c>
-      <c r="C36" t="s"/>
-      <c r="D36" t="s"/>
-      <c r="E36" t="s"/>
+      <c r="C36" t="inlineStr"/>
+      <c r="D36" t="inlineStr"/>
+      <c r="E36" t="inlineStr"/>
       <c r="F36" t="n">
         <v>0.09386045796834179</v>
       </c>
@@ -1661,16 +1660,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:12">
-      <c r="A37" s="1" t="s">
-        <v>48</v>
+    <row r="37">
+      <c r="A37" s="1" t="inlineStr">
+        <is>
+          <t>fire</t>
+        </is>
       </c>
       <c r="B37" t="n">
         <v>26028</v>
       </c>
-      <c r="C37" t="s"/>
-      <c r="D37" t="s"/>
-      <c r="E37" t="s"/>
+      <c r="C37" t="inlineStr"/>
+      <c r="D37" t="inlineStr"/>
+      <c r="E37" t="inlineStr"/>
       <c r="F37" t="n">
         <v>0.01083448593822038</v>
       </c>
@@ -1693,16 +1694,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:12">
-      <c r="A38" s="1" t="s">
-        <v>49</v>
+    <row r="38">
+      <c r="A38" s="1" t="inlineStr">
+        <is>
+          <t>earthquake</t>
+        </is>
       </c>
       <c r="B38" t="n">
         <v>26028</v>
       </c>
-      <c r="C38" t="s"/>
-      <c r="D38" t="s"/>
-      <c r="E38" t="s"/>
+      <c r="C38" t="inlineStr"/>
+      <c r="D38" t="inlineStr"/>
+      <c r="E38" t="inlineStr"/>
       <c r="F38" t="n">
         <v>0.09432149992315968</v>
       </c>
@@ -1725,16 +1728,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:12">
-      <c r="A39" s="1" t="s">
-        <v>50</v>
+    <row r="39">
+      <c r="A39" s="1" t="inlineStr">
+        <is>
+          <t>cold</t>
+        </is>
       </c>
       <c r="B39" t="n">
         <v>26028</v>
       </c>
-      <c r="C39" t="s"/>
-      <c r="D39" t="s"/>
-      <c r="E39" t="s"/>
+      <c r="C39" t="inlineStr"/>
+      <c r="D39" t="inlineStr"/>
+      <c r="E39" t="inlineStr"/>
       <c r="F39" t="n">
         <v>0.02036268633779007</v>
       </c>
@@ -1757,16 +1762,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:12">
-      <c r="A40" s="1" t="s">
-        <v>51</v>
+    <row r="40">
+      <c r="A40" s="1" t="inlineStr">
+        <is>
+          <t>other_weather</t>
+        </is>
       </c>
       <c r="B40" t="n">
         <v>26028</v>
       </c>
-      <c r="C40" t="s"/>
-      <c r="D40" t="s"/>
-      <c r="E40" t="s"/>
+      <c r="C40" t="inlineStr"/>
+      <c r="D40" t="inlineStr"/>
+      <c r="E40" t="inlineStr"/>
       <c r="F40" t="n">
         <v>0.05286614415245121</v>
       </c>
@@ -1789,16 +1796,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:12">
-      <c r="A41" s="1" t="s">
-        <v>52</v>
+    <row r="41">
+      <c r="A41" s="1" t="inlineStr">
+        <is>
+          <t>direct_report</t>
+        </is>
       </c>
       <c r="B41" t="n">
         <v>26028</v>
       </c>
-      <c r="C41" t="s"/>
-      <c r="D41" t="s"/>
-      <c r="E41" t="s"/>
+      <c r="C41" t="inlineStr"/>
+      <c r="D41" t="inlineStr"/>
+      <c r="E41" t="inlineStr"/>
       <c r="F41" t="n">
         <v>0.1949823267250653</v>
       </c>

</xml_diff>